<commit_message>
server: matching용 스레드 추가
matching 요청이 과도하게 들어오면 기아현상이 발생하는것 같아서 따로 만듦
</commit_message>
<xml_diff>
--- a/Server/Server/GameData/Map.xlsx
+++ b/Server/Server/GameData/Map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\FestivalTownProject\Client\Assets\11. GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A1BB10-64D0-4ED9-A241-0AA75CAE2741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8922CA20-88DB-419D-9E0E-EA0C0E33DB01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23250" yWindow="2295" windowWidth="22680" windowHeight="11295" activeTab="1" xr2:uid="{921AD0DD-2680-48BD-95A5-710096326966}"/>
+    <workbookView xWindow="-26355" yWindow="2820" windowWidth="22680" windowHeight="11295" activeTab="1" xr2:uid="{921AD0DD-2680-48BD-95A5-710096326966}"/>
   </bookViews>
   <sheets>
     <sheet name="Theme" sheetId="2" r:id="rId1"/>
@@ -260,10 +260,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Statue_Team_Red_LocationX </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Statue_Team_Red_LocationZ</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -280,26 +276,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Statue_Team_Blue_LocationX </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Statue_Team_Blue_LocationZ</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Statue_Team_Green_LocationX </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Statue_Team_Green_LocationZ</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Statue_Team_Red_LocationY </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Statue_Team_Blue_LocationY</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -348,7 +332,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Index </t>
+    <t>Index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Statue_Team_Red_LocationX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Statue_Team_Red_LocationY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Statue_Team_Blue_LocationX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Statue_Team_Green_LocationX</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -356,7 +356,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -388,12 +388,6 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -853,7 +847,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -869,25 +863,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -898,19 +892,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="G2" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -921,19 +915,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="G3" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -944,19 +938,19 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -967,19 +961,19 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="G5" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -990,19 +984,19 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="G6" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1013,19 +1007,19 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="G7" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1036,19 +1030,19 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="G8" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1059,19 +1053,19 @@
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="G9" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1086,7 +1080,7 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1111,7 +1105,7 @@
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1132,40 +1126,40 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
server: pass data load 수정 / pass용 db 쿼리문 추가
</commit_message>
<xml_diff>
--- a/Server/Server/GameData/Map.xlsx
+++ b/Server/Server/GameData/Map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FestivalTownProject\Client\Assets\11. GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDDE9A6-0F64-41F8-8E42-E2883A6D3470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB592668-FD4D-4D42-A3AC-B75F0384057D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="1420" windowWidth="21600" windowHeight="11180" activeTab="1" xr2:uid="{921AD0DD-2680-48BD-95A5-710096326966}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{921AD0DD-2680-48BD-95A5-710096326966}"/>
   </bookViews>
   <sheets>
     <sheet name="Theme" sheetId="2" r:id="rId1"/>
@@ -1495,8 +1495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B9C196F-4F00-40D9-AF4A-152034752A4E}">
   <dimension ref="A1:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2191,7 +2191,7 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -2200,7 +2200,7 @@
         <v>26</v>
       </c>
       <c r="K12">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="L12">
         <v>0</v>

</xml_diff>